<commit_message>
format laporan modul 2
</commit_message>
<xml_diff>
--- a/Kelompok Praktikum MDP 2018.xlsx
+++ b/Kelompok Praktikum MDP 2018.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vizya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Undip\Semester 7\Git asisten\Keperluan-Praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A01D0-2430-4BD9-8F7A-13CB4FB8BE5C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94394F97-5C24-46A8-979B-50A5F9F9AE49}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{18BCE4B8-E7B1-4F8D-AAEE-675CE965675A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>VERONIKA PUTRI INDAH BESTARI</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>13.15 - 15.45</t>
+  </si>
+  <si>
+    <t>minus</t>
+  </si>
+  <si>
+    <t>ga dateng</t>
+  </si>
+  <si>
+    <t>izin</t>
   </si>
 </sst>
 </file>
@@ -478,19 +487,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,6 +512,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -824,46 +833,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6E757C-D704-4F2D-9B27-0FB2A1953735}">
   <dimension ref="B2:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>21120116130044</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>21120116130066</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>85</v>
       </c>
@@ -871,17 +883,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>21120116120024</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="9">
         <v>2</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="11"/>
       <c r="G4" s="3" t="s">
         <v>86</v>
       </c>
@@ -889,15 +901,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>21120116120009</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
       <c r="G5" s="3" t="s">
         <v>88</v>
       </c>
@@ -905,902 +917,962 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>21120116130052</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="9">
         <v>3</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>21120116120010</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>21120116130073</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="9">
         <v>4</v>
       </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>21120116120012</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>21120116120003</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>5</v>
       </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>21120116130060</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="8"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>21120116140068</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>6</v>
       </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>21120116140051</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>21120116130042</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="9">
         <v>7</v>
       </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>21120116130065</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>21120116130049</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="9">
         <v>8</v>
       </c>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>21120116120017</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>21120116120029</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="9">
         <v>9</v>
       </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>21120116140045</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>21120116120005</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="9">
         <v>10</v>
       </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>21120116120006</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>21120116140078</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="9">
         <v>11</v>
       </c>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>21120116140034</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>21120116130036</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="9">
         <v>12</v>
       </c>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>21120116140053</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>21120116120027</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="9">
         <v>13</v>
       </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>21120116140072</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>21120112140088</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="9">
         <v>14</v>
       </c>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>21120116120028</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>21120116120013</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="9">
         <v>15</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>21120116120016</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D31" s="10"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>21120116140039</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="9">
         <v>16</v>
       </c>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>21120114130086</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D33" s="10"/>
+      <c r="E33" s="12"/>
+      <c r="F33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>21120116140062</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="9">
         <v>17</v>
       </c>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>21120116130063</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="13"/>
-    </row>
-    <row r="36" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D35" s="10"/>
+      <c r="E35" s="12"/>
+      <c r="F35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>21120116120025</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="9">
         <v>18</v>
       </c>
-      <c r="E36" s="13"/>
-    </row>
-    <row r="37" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>21120116120018</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="13"/>
-    </row>
-    <row r="38" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D37" s="10"/>
+      <c r="E37" s="12"/>
+      <c r="F37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>21120116120033</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="9">
         <v>19</v>
       </c>
-      <c r="E38" s="13"/>
-    </row>
-    <row r="39" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>21120116130076</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="13"/>
-    </row>
-    <row r="40" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D39" s="10"/>
+      <c r="E39" s="12"/>
+      <c r="F39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>21120116120011</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="9">
         <v>20</v>
       </c>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>21120116130035</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D41" s="10"/>
+      <c r="E41" s="12"/>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>21120116120020</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="9">
         <v>21</v>
       </c>
-      <c r="E42" s="13"/>
-    </row>
-    <row r="43" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E42" s="12"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>21120116120026</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="13"/>
-    </row>
-    <row r="44" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D43" s="10"/>
+      <c r="E43" s="12"/>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>21120116130041</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="9">
         <v>22</v>
       </c>
-      <c r="E44" s="13"/>
-    </row>
-    <row r="45" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>21120116130075</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="13"/>
-    </row>
-    <row r="46" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D45" s="10"/>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>21120116120032</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="9">
         <v>23</v>
       </c>
-      <c r="E46" s="13"/>
-    </row>
-    <row r="47" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>21120116120019</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="13"/>
-    </row>
-    <row r="48" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D47" s="10"/>
+      <c r="E47" s="12"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>21120116120014</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="9">
         <v>24</v>
       </c>
-      <c r="E48" s="13"/>
-    </row>
-    <row r="49" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E48" s="12"/>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>21120116120022</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="13"/>
-    </row>
-    <row r="50" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D49" s="10"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>21120112140027</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="9">
         <v>25</v>
       </c>
-      <c r="E50" s="13"/>
-    </row>
-    <row r="51" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>21120112130019</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="13"/>
-    </row>
-    <row r="52" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D51" s="10"/>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>21120116120015</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="9">
         <v>26</v>
       </c>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>21120116140088</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="13"/>
-    </row>
-    <row r="54" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D53" s="10"/>
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>21120116120002</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="9">
         <v>27</v>
       </c>
-      <c r="E54" s="13"/>
-    </row>
-    <row r="55" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>21120116120021</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="13"/>
-    </row>
-    <row r="56" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D55" s="10"/>
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
         <v>21120116140038</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="9">
         <v>28</v>
       </c>
-      <c r="E56" s="13"/>
-    </row>
-    <row r="57" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
         <v>21120116130043</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="13"/>
-    </row>
-    <row r="58" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D57" s="10"/>
+      <c r="E57" s="12"/>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>21120116140077</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="9">
         <v>29</v>
       </c>
-      <c r="E58" s="14">
+      <c r="E58" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>21120116120004</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="15"/>
-    </row>
-    <row r="60" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D59" s="10"/>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>21120116120007</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="9">
         <v>30</v>
       </c>
-      <c r="E60" s="15"/>
-    </row>
-    <row r="61" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>21120116140081</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="15"/>
-    </row>
-    <row r="62" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D61" s="10"/>
+      <c r="E61" s="14"/>
+      <c r="F61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>21120116130057</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="9">
         <v>31</v>
       </c>
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E62" s="14"/>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>21120116140083</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D63" s="10"/>
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>21120116130082</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="9">
         <v>32</v>
       </c>
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E64" s="14"/>
+      <c r="F64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>21120116130056</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="15"/>
-    </row>
-    <row r="66" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D65" s="16"/>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>21120116130047</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="9">
         <v>33</v>
       </c>
-      <c r="E66" s="15"/>
-    </row>
-    <row r="67" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E66" s="14"/>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>21120116140054</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D67" s="10"/>
+      <c r="E67" s="14"/>
+      <c r="F67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>21120116130037</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="9">
         <v>34</v>
       </c>
-      <c r="E68" s="15"/>
-    </row>
-    <row r="69" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E68" s="14"/>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>21120116140087</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="15"/>
-    </row>
-    <row r="70" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D69" s="10"/>
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
         <v>21120116130059</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D70" s="9">
         <v>35</v>
       </c>
-      <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E70" s="14"/>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>21120116130084</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="15"/>
-    </row>
-    <row r="72" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D71" s="10"/>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
         <v>21120116130048</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="9">
         <v>36</v>
       </c>
-      <c r="E72" s="15"/>
-    </row>
-    <row r="73" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E72" s="14"/>
+    </row>
+    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="1">
         <v>21120116130086</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D73" s="10"/>
+      <c r="E73" s="14"/>
+      <c r="F73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="1">
         <v>21120116120008</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="9">
         <v>37</v>
       </c>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E74" s="14"/>
+    </row>
+    <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="1">
         <v>21120116140058</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D75" s="8"/>
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D75" s="10"/>
+      <c r="E75" s="14"/>
+    </row>
+    <row r="76" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
         <v>21120116130046</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="9">
         <v>38</v>
       </c>
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E76" s="14"/>
+    </row>
+    <row r="77" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="1">
         <v>21120116130061</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D77" s="8"/>
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D77" s="10"/>
+      <c r="E77" s="14"/>
+    </row>
+    <row r="78" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="1">
         <v>21120116120031</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="9">
         <v>39</v>
       </c>
-      <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E78" s="14"/>
+    </row>
+    <row r="79" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="1">
         <v>21120116130067</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D79" s="8"/>
-      <c r="E79" s="15"/>
-    </row>
-    <row r="80" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D79" s="10"/>
+      <c r="E79" s="14"/>
+    </row>
+    <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
         <v>21120116140071</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="9">
         <v>40</v>
       </c>
-      <c r="E80" s="15"/>
-    </row>
-    <row r="81" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E80" s="14"/>
+    </row>
+    <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
         <v>21120116130080</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D81" s="9"/>
-      <c r="E81" s="15"/>
-    </row>
-    <row r="82" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D81" s="16"/>
+      <c r="E81" s="14"/>
+      <c r="F81" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>21120116140070</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D82" s="11">
+      <c r="D82" s="8">
         <v>41</v>
       </c>
-      <c r="E82" s="15"/>
-    </row>
-    <row r="83" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E82" s="14"/>
+    </row>
+    <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
         <v>21120116140069</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D83" s="11"/>
-      <c r="E83" s="15"/>
-    </row>
-    <row r="84" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D83" s="8"/>
+      <c r="E83" s="14"/>
+    </row>
+    <row r="84" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4">
         <v>21120116140074</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D84" s="11">
+      <c r="D84" s="8">
         <v>42</v>
       </c>
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E84" s="14"/>
+    </row>
+    <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>21120116140050</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D85" s="11"/>
-      <c r="E85" s="15"/>
-    </row>
-    <row r="86" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D85" s="8"/>
+      <c r="E85" s="14"/>
+    </row>
+    <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="4">
         <v>21120113140091</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="16"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="15"/>
+      <c r="F86" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="D82:D83"/>
     <mergeCell ref="D84:D86"/>
@@ -1817,36 +1889,6 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="D80:D81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>